<commit_message>
update lector de .txt
</commit_message>
<xml_diff>
--- a/archivos.xlsx
+++ b/archivos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell_Sudcompu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PHPProjects\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,32 +32,37 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>MK-5N</t>
-  </si>
-  <si>
     <t>TEST1</t>
   </si>
   <si>
-    <t>MK-7N</t>
-  </si>
-  <si>
     <t>TESST2</t>
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>00000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,7 +371,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,35 +381,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>